<commit_message>
[feature] correcion de mostrar los datos de la empresa y correccion del documento de excel
</commit_message>
<xml_diff>
--- a/src/assets/anexos/creditos_preaprobados_empleados_v_ifis.xlsx
+++ b/src/assets/anexos/creditos_preaprobados_empleados_v_ifis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/coop-ifi-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186E21D1-859F-B944-B6F9-294759EC0364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA176E8-B6CD-F24F-913C-2A9E2D4FFB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -139,6 +139,7 @@
         <sz val="11"/>
         <color indexed="11"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>jimmy1817@hotmail.com</t>
     </r>
@@ -168,12 +169,14 @@
       <sz val="11"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -218,30 +221,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1405,15 +1407,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="10.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="20" width="17.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="11" customWidth="1"/>
+    <col min="2" max="8" width="10.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="10" customWidth="1"/>
+    <col min="10" max="17" width="17.1640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" style="10" customWidth="1"/>
+    <col min="19" max="20" width="17.1640625" style="1" customWidth="1"/>
     <col min="21" max="21" width="27.83203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="31.6640625" style="1" customWidth="1"/>
     <col min="23" max="23" width="29.6640625" style="1" customWidth="1"/>
@@ -1422,7 +1427,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1520,41 +1525,41 @@
       <c r="I2" s="5">
         <v>1003150603</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <v>36161</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="9"/>
+      <c r="T2" s="8"/>
       <c r="U2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="W2" s="2" t="s">
@@ -1589,41 +1594,41 @@
       <c r="I3" s="5">
         <v>1003150602</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>36161</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="9"/>
+      <c r="T3" s="8"/>
       <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="W3" s="2" t="s">

</xml_diff>

<commit_message>
[Abraham]: Fixed name enterprise in file for send email.
</commit_message>
<xml_diff>
--- a/src/assets/anexos/creditos_preaprobados_empleados_v_ifis.xlsx
+++ b/src/assets/anexos/creditos_preaprobados_empleados_v_ifis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/coop-ifi-front-center/src/assets/anexos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Desktop/Project/BigPuntos/Front/coop-ifi-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA176E8-B6CD-F24F-913C-2A9E2D4FFB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92079E8-7B9B-CE49-A372-F80924EFA194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>1002003004003</t>
   </si>
   <si>
-    <t>Mutualista Imbabura</t>
-  </si>
-  <si>
     <t>1002003004001,1002003004002</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   <si>
     <t>abraham-rat@outlook.es</t>
   </si>
+  <si>
+    <t>Cooperativa de Ahorro y Crédito San José de Vittoria</t>
+  </si>
 </sst>
 </file>
 
@@ -158,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -175,6 +175,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -221,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -244,6 +250,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1408,7 +1417,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1547,7 +1556,7 @@
         <v>31</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>32</v>
@@ -1559,11 +1568,11 @@
       <c r="U2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1595,7 +1604,7 @@
         <v>1003150602</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>27</v>
@@ -1616,23 +1625,23 @@
         <v>31</v>
       </c>
       <c r="Q3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="S3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T3" s="8"/>
       <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>